<commit_message>
update ledger and maintain connection
</commit_message>
<xml_diff>
--- a/xlsx_template/data.xlsx
+++ b/xlsx_template/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15120" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37148" uniqueCount="400">
   <si>
     <t>CXD</t>
   </si>
@@ -1248,6 +1248,21 @@
   <si>
     <t>6000</t>
   </si>
+  <si>
+    <t>280000</t>
+  </si>
+  <si>
+    <t>560000</t>
+  </si>
+  <si>
+    <t>720000</t>
+  </si>
+  <si>
+    <t>129232</t>
+  </si>
+  <si>
+    <t>320000</t>
+  </si>
 </sst>
 </file>
 
@@ -2560,76 +2575,76 @@
       <c r="J7" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="K7" t="s" s="10">
+      <c r="K7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s" s="10">
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="M7" t="s" s="10">
+      <c r="M7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s" s="10">
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="O7" t="s" s="10">
+      <c r="O7" t="s">
         <v>26</v>
       </c>
-      <c r="P7" t="s" s="10">
+      <c r="P7" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" t="s" s="10">
+      <c r="Q7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" t="s" s="10">
+      <c r="R7" t="s">
         <v>26</v>
       </c>
-      <c r="S7" t="s" s="10">
+      <c r="S7" t="s">
         <v>26</v>
       </c>
-      <c r="T7" t="s" s="10">
+      <c r="T7" t="s">
         <v>26</v>
       </c>
-      <c r="U7" t="s" s="10">
+      <c r="U7" t="s">
         <v>26</v>
       </c>
-      <c r="V7" t="s" s="10">
+      <c r="V7" t="s">
         <v>27</v>
       </c>
-      <c r="W7" t="s" s="10">
+      <c r="W7" t="s">
         <v>27</v>
       </c>
-      <c r="X7" t="s" s="10">
+      <c r="X7" t="s">
         <v>27</v>
       </c>
-      <c r="Y7" t="s" s="10">
+      <c r="Y7" t="s">
         <v>27</v>
       </c>
-      <c r="Z7" t="s" s="10">
+      <c r="Z7" t="s">
         <v>27</v>
       </c>
-      <c r="AA7" t="s" s="10">
+      <c r="AA7" t="s">
         <v>27</v>
       </c>
-      <c r="AB7" t="s" s="10">
+      <c r="AB7" t="s">
         <v>27</v>
       </c>
-      <c r="AC7" t="s" s="10">
+      <c r="AC7" t="s">
         <v>27</v>
       </c>
-      <c r="AD7" t="s" s="10">
+      <c r="AD7" t="s">
         <v>27</v>
       </c>
-      <c r="AE7" t="s" s="10">
+      <c r="AE7" t="s">
         <v>27</v>
       </c>
-      <c r="AF7" t="s" s="10">
+      <c r="AF7" t="s">
         <v>27</v>
       </c>
-      <c r="AG7" t="s" s="10">
+      <c r="AG7" t="s">
         <v>27</v>
       </c>
-      <c r="AH7" t="s" s="10">
+      <c r="AH7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2640,76 +2655,76 @@
       <c r="J8" t="s" s="10">
         <v>0</v>
       </c>
-      <c r="K8" t="s" s="10">
+      <c r="K8" t="s">
         <v>95</v>
       </c>
-      <c r="L8" t="s" s="10">
+      <c r="L8" t="s">
         <v>96</v>
       </c>
-      <c r="M8" t="s" s="10">
+      <c r="M8" t="s">
         <v>97</v>
       </c>
-      <c r="N8" t="s" s="10">
+      <c r="N8" t="s">
         <v>1</v>
       </c>
-      <c r="O8" t="s" s="10">
+      <c r="O8" t="s">
         <v>98</v>
       </c>
-      <c r="P8" t="s" s="10">
+      <c r="P8" t="s">
         <v>2</v>
       </c>
-      <c r="Q8" t="s" s="10">
+      <c r="Q8" t="s">
         <v>99</v>
       </c>
-      <c r="R8" t="s" s="10">
+      <c r="R8" t="s">
         <v>3</v>
       </c>
-      <c r="S8" t="s" s="10">
+      <c r="S8" t="s">
         <v>100</v>
       </c>
-      <c r="T8" t="s" s="10">
+      <c r="T8" t="s">
         <v>101</v>
       </c>
-      <c r="U8" t="s" s="10">
+      <c r="U8" t="s">
         <v>102</v>
       </c>
-      <c r="V8" t="s" s="10">
+      <c r="V8" t="s">
         <v>94</v>
       </c>
-      <c r="W8" t="s" s="10">
+      <c r="W8" t="s">
         <v>0</v>
       </c>
-      <c r="X8" t="s" s="10">
+      <c r="X8" t="s">
         <v>95</v>
       </c>
-      <c r="Y8" t="s" s="10">
+      <c r="Y8" t="s">
         <v>96</v>
       </c>
-      <c r="Z8" t="s" s="10">
+      <c r="Z8" t="s">
         <v>97</v>
       </c>
-      <c r="AA8" t="s" s="10">
+      <c r="AA8" t="s">
         <v>1</v>
       </c>
-      <c r="AB8" t="s" s="10">
+      <c r="AB8" t="s">
         <v>98</v>
       </c>
-      <c r="AC8" t="s" s="10">
+      <c r="AC8" t="s">
         <v>2</v>
       </c>
-      <c r="AD8" t="s" s="10">
+      <c r="AD8" t="s">
         <v>99</v>
       </c>
-      <c r="AE8" t="s" s="10">
+      <c r="AE8" t="s">
         <v>3</v>
       </c>
-      <c r="AF8" t="s" s="10">
+      <c r="AF8" t="s">
         <v>100</v>
       </c>
-      <c r="AG8" t="s" s="10">
+      <c r="AG8" t="s">
         <v>101</v>
       </c>
-      <c r="AH8" t="s" s="10">
+      <c r="AH8" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2727,13 +2742,13 @@
         <v>28</v>
       </c>
       <c r="F9" t="s" s="10">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="G9" t="s" s="10">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="H9" t="s" s="10">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="I9" t="s" s="10">
         <v>268</v>
@@ -2754,13 +2769,13 @@
         <v>234</v>
       </c>
       <c r="O9" t="s" s="10">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="P9" t="s" s="10">
         <v>234</v>
       </c>
       <c r="Q9" t="s" s="10">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="R9" t="s" s="10">
         <v>234</v>
@@ -2843,13 +2858,13 @@
         <v>28</v>
       </c>
       <c r="F10" t="s" s="10">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="G10" t="s" s="10">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="H10" t="s" s="10">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="I10" t="s" s="10">
         <v>268</v>
@@ -2870,13 +2885,13 @@
         <v>234</v>
       </c>
       <c r="O10" t="s" s="10">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="P10" t="s" s="10">
         <v>234</v>
       </c>
       <c r="Q10" t="s" s="10">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="R10" t="s" s="10">
         <v>234</v>
@@ -2959,13 +2974,13 @@
         <v>4</v>
       </c>
       <c r="F11" t="s" s="10">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="G11" t="s" s="10">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="H11" t="s" s="10">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="I11" t="s" s="10">
         <v>234</v>
@@ -2986,13 +3001,13 @@
         <v>234</v>
       </c>
       <c r="O11" t="s" s="10">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="P11" t="s" s="10">
         <v>234</v>
       </c>
       <c r="Q11" t="s" s="10">
-        <v>234</v>
+        <v>389</v>
       </c>
       <c r="R11" t="s" s="10">
         <v>234</v>
@@ -3191,13 +3206,13 @@
         <v>31</v>
       </c>
       <c r="F13" t="s" s="10">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G13" t="s" s="10">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H13" t="s" s="10">
-        <v>237</v>
+        <v>399</v>
       </c>
       <c r="I13" t="s" s="10">
         <v>234</v>
@@ -3218,13 +3233,13 @@
         <v>234</v>
       </c>
       <c r="O13" t="s" s="10">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="P13" t="s" s="10">
         <v>234</v>
       </c>
       <c r="Q13" t="s" s="10">
-        <v>234</v>
+        <v>389</v>
       </c>
       <c r="R13" t="s" s="10">
         <v>234</v>
@@ -4344,76 +4359,76 @@
       <c r="J24" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="K24" t="s" s="10">
+      <c r="K24" t="s">
         <v>26</v>
       </c>
-      <c r="L24" t="s" s="10">
+      <c r="L24" t="s">
         <v>26</v>
       </c>
-      <c r="M24" t="s" s="10">
+      <c r="M24" t="s">
         <v>26</v>
       </c>
-      <c r="N24" t="s" s="10">
+      <c r="N24" t="s">
         <v>26</v>
       </c>
-      <c r="O24" t="s" s="10">
+      <c r="O24" t="s">
         <v>26</v>
       </c>
-      <c r="P24" t="s" s="10">
+      <c r="P24" t="s">
         <v>26</v>
       </c>
-      <c r="Q24" t="s" s="10">
+      <c r="Q24" t="s">
         <v>26</v>
       </c>
-      <c r="R24" t="s" s="10">
+      <c r="R24" t="s">
         <v>26</v>
       </c>
-      <c r="S24" t="s" s="10">
+      <c r="S24" t="s">
         <v>26</v>
       </c>
-      <c r="T24" t="s" s="10">
+      <c r="T24" t="s">
         <v>26</v>
       </c>
-      <c r="U24" t="s" s="10">
+      <c r="U24" t="s">
         <v>26</v>
       </c>
-      <c r="V24" t="s" s="10">
+      <c r="V24" t="s">
         <v>27</v>
       </c>
-      <c r="W24" t="s" s="10">
+      <c r="W24" t="s">
         <v>27</v>
       </c>
-      <c r="X24" t="s" s="10">
+      <c r="X24" t="s">
         <v>27</v>
       </c>
-      <c r="Y24" t="s" s="10">
+      <c r="Y24" t="s">
         <v>27</v>
       </c>
-      <c r="Z24" t="s" s="10">
+      <c r="Z24" t="s">
         <v>27</v>
       </c>
-      <c r="AA24" t="s" s="10">
+      <c r="AA24" t="s">
         <v>27</v>
       </c>
-      <c r="AB24" t="s" s="10">
+      <c r="AB24" t="s">
         <v>27</v>
       </c>
-      <c r="AC24" t="s" s="10">
+      <c r="AC24" t="s">
         <v>27</v>
       </c>
-      <c r="AD24" t="s" s="10">
+      <c r="AD24" t="s">
         <v>27</v>
       </c>
-      <c r="AE24" t="s" s="10">
+      <c r="AE24" t="s">
         <v>27</v>
       </c>
-      <c r="AF24" t="s" s="10">
+      <c r="AF24" t="s">
         <v>27</v>
       </c>
-      <c r="AG24" t="s" s="10">
+      <c r="AG24" t="s">
         <v>27</v>
       </c>
-      <c r="AH24" t="s" s="10">
+      <c r="AH24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4424,76 +4439,76 @@
       <c r="J25" t="s" s="10">
         <v>0</v>
       </c>
-      <c r="K25" t="s" s="10">
+      <c r="K25" t="s">
         <v>95</v>
       </c>
-      <c r="L25" t="s" s="10">
+      <c r="L25" t="s">
         <v>96</v>
       </c>
-      <c r="M25" t="s" s="10">
+      <c r="M25" t="s">
         <v>97</v>
       </c>
-      <c r="N25" t="s" s="10">
+      <c r="N25" t="s">
         <v>1</v>
       </c>
-      <c r="O25" t="s" s="10">
+      <c r="O25" t="s">
         <v>98</v>
       </c>
-      <c r="P25" t="s" s="10">
+      <c r="P25" t="s">
         <v>2</v>
       </c>
-      <c r="Q25" t="s" s="10">
+      <c r="Q25" t="s">
         <v>99</v>
       </c>
-      <c r="R25" t="s" s="10">
+      <c r="R25" t="s">
         <v>3</v>
       </c>
-      <c r="S25" t="s" s="10">
+      <c r="S25" t="s">
         <v>100</v>
       </c>
-      <c r="T25" t="s" s="10">
+      <c r="T25" t="s">
         <v>101</v>
       </c>
-      <c r="U25" t="s" s="10">
+      <c r="U25" t="s">
         <v>102</v>
       </c>
-      <c r="V25" t="s" s="10">
+      <c r="V25" t="s">
         <v>94</v>
       </c>
-      <c r="W25" t="s" s="10">
+      <c r="W25" t="s">
         <v>0</v>
       </c>
-      <c r="X25" t="s" s="10">
+      <c r="X25" t="s">
         <v>95</v>
       </c>
-      <c r="Y25" t="s" s="10">
+      <c r="Y25" t="s">
         <v>96</v>
       </c>
-      <c r="Z25" t="s" s="10">
+      <c r="Z25" t="s">
         <v>97</v>
       </c>
-      <c r="AA25" t="s" s="10">
+      <c r="AA25" t="s">
         <v>1</v>
       </c>
-      <c r="AB25" t="s" s="10">
+      <c r="AB25" t="s">
         <v>98</v>
       </c>
-      <c r="AC25" t="s" s="10">
+      <c r="AC25" t="s">
         <v>2</v>
       </c>
-      <c r="AD25" t="s" s="10">
+      <c r="AD25" t="s">
         <v>99</v>
       </c>
-      <c r="AE25" t="s" s="10">
+      <c r="AE25" t="s">
         <v>3</v>
       </c>
-      <c r="AF25" t="s" s="10">
+      <c r="AF25" t="s">
         <v>100</v>
       </c>
-      <c r="AG25" t="s" s="10">
+      <c r="AG25" t="s">
         <v>101</v>
       </c>
-      <c r="AH25" t="s" s="10">
+      <c r="AH25" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>